<commit_message>
Acrescentado exemplo de Backlog, att
</commit_message>
<xml_diff>
--- a/SprintBacklog (modelo exemplo).xlsx
+++ b/SprintBacklog (modelo exemplo).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markz\Desktop\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A75B576F-1B91-4926-98C8-41B7DDC26701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB191DC6-5E2C-4EA8-8174-C6B7F94FF4D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9A331121-C00D-4716-8A12-865F1F91B6B6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t xml:space="preserve">Modelo de Sprint Backlog </t>
   </si>
@@ -72,22 +72,7 @@
     <t>Revisão do Sprint</t>
   </si>
   <si>
-    <t>História de Usuário #1</t>
-  </si>
-  <si>
     <t>Tarefa</t>
-  </si>
-  <si>
-    <t>História de Usuário #2</t>
-  </si>
-  <si>
-    <t>História de Usuário #3</t>
-  </si>
-  <si>
-    <t>História de Usuário #4</t>
-  </si>
-  <si>
-    <t>História de Usuário #5</t>
   </si>
   <si>
     <t>Total</t>
@@ -97,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,15 +96,8 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,12 +113,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -188,19 +160,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1222,13 +1186,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1613,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50801E37-6109-446F-9593-C428D7E1B4D3}">
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,7 +1588,7 @@
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1734,7 +1698,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="8"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1784,20 +1748,20 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1809,19 +1773,19 @@
       <c r="T7" s="1"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1833,19 +1797,19 @@
       <c r="T8" s="1"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1857,19 +1821,19 @@
       <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1881,19 +1845,19 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1904,20 +1868,20 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1929,19 +1893,19 @@
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1953,19 +1917,19 @@
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1977,19 +1941,19 @@
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
+      <c r="A15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -2001,19 +1965,19 @@
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -2024,20 +1988,20 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -2049,19 +2013,19 @@
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
+      <c r="A18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -2073,19 +2037,19 @@
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
+      <c r="A19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -2097,19 +2061,19 @@
       <c r="T19" s="1"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
+      <c r="A20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -2121,19 +2085,19 @@
       <c r="T20" s="1"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
+      <c r="A21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -2144,20 +2108,20 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -2169,19 +2133,19 @@
       <c r="T22" s="1"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
+      <c r="A23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -2193,19 +2157,19 @@
       <c r="T23" s="1"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
+      <c r="A24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -2217,19 +2181,19 @@
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
+      <c r="A25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -2241,19 +2205,19 @@
       <c r="T25" s="1"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
+      <c r="A26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -2264,20 +2228,41 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="6"/>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="E27" s="7">
+        <f>SUM(E7:E26)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="7">
+        <f>SUM(F7:F26)</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="7">
+        <f>SUM(G7:G26)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="7">
+        <f>SUM(H7:H26)</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="7">
+        <f>SUM(I7:I26)</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="7">
+        <f>SUM(J7:J26)</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="7">
+        <f>SUM(K7:K26)</f>
+        <v>0</v>
+      </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -2288,147 +2273,6 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11">
-        <f>SUM(E7:E31)</f>
-        <v>0</v>
-      </c>
-      <c r="F32" s="11">
-        <f>SUM(F8:F31)</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="11">
-        <f>SUM(G7:G31)</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="11">
-        <f>SUM(H7:H31)</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="11">
-        <f>SUM(I7:I31)</f>
-        <v>0</v>
-      </c>
-      <c r="J32" s="11">
-        <f>SUM(J7:J31)</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="11">
-        <f>SUM(K7:K31)</f>
-        <v>0</v>
-      </c>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>